<commit_message>
Moved "Ser/Plas^donor" to group "BldSerPlas^donor"
</commit_message>
<xml_diff>
--- a/class_MICRO/system_groupings.xlsx
+++ b/class_MICRO/system_groupings.xlsx
@@ -16280,8 +16280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="I132" sqref="I132"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="H118" sqref="H118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.85546875" defaultRowHeight="15"/>
@@ -19491,7 +19491,7 @@
         <v>4122</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>3707</v>
+        <v>3742</v>
       </c>
       <c r="L117" s="1" t="s">
         <v>4123</v>

</xml_diff>